<commit_message>
added line of best fit
</commit_message>
<xml_diff>
--- a/application/data/covid19_app_country_agnostic_dataset.xlsx
+++ b/application/data/covid19_app_country_agnostic_dataset.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\University\COM618-DataScience\application\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4DA8B23-B74D-434A-A441-12AC0E3EEB0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{67741318-6BB6-42AF-B43A-80CFB8C4DA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_app_country_agnostic_da" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="10" uniqueCount="10">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="11" uniqueCount="11">
   <si>
     <t>Week starting</t>
   </si>
@@ -67,11 +67,14 @@
   <si>
     <t>Deaths</t>
   </si>
+  <si>
+    <t>Date</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -644,6 +647,971 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://purl.oclc.org/ooxml/drawingml/chart" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0%">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65%"/>
+                  <a:lumOff val="35%"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>DeathsAgainstDownloadPerMonth!$A$2:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>44044</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44136</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44166</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44197</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44228</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44287</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44317</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44348</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44378</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44409</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44440</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44470</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44501</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44531</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44562</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>DeathsAgainstDownloadPerMonth!$C$2:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>297</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>605</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3507</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8660</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10678</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19625</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9532</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2853</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>713</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>273</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>329</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1218</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2346</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2741</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2809</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2958</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4292</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1CCA-49EC-B7F6-7C28AC986731}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="2074354864"/>
+        <c:axId val="2074355696"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="2074354864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15%"/>
+                <a:lumOff val="85%"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65%"/>
+                    <a:lumOff val="35%"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2074355696"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="2074355696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15%"/>
+                  <a:lumOff val="85%"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0%">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65%"/>
+                    <a:lumOff val="35%"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2074354864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15%"/>
+          <a:lumOff val="85%"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80%"/>
+    <a:lumOff val="20%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60%"/>
+    <a:lumOff val="40%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70%"/>
+    <a:lumOff val="30%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70%"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50%"/>
+    <a:lumOff val="50%"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15%"/>
+            <a:lumOff val="85%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15%"/>
+            <a:lumOff val="85%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75%"/>
+        <a:lumOff val="25%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25%"/>
+            <a:lumOff val="75%"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15%"/>
+            <a:lumOff val="85%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65%"/>
+          <a:lumOff val="35%"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65%"/>
+            <a:lumOff val="35%"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35%"/>
+            <a:lumOff val="65%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65%"/>
+            <a:lumOff val="35%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15%"/>
+            <a:lumOff val="85%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5%"/>
+            <a:lumOff val="95%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75%"/>
+            <a:lumOff val="25%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35%"/>
+            <a:lumOff val="65%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35%"/>
+            <a:lumOff val="65%"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0%"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15%"/>
+            <a:lumOff val="85%"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65%"/>
+        <a:lumOff val="35%"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1B34F96-C399-45C2-BCDB-1C463636F756}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://purl.oclc.org/ooxml/drawingml/chart">
+          <c:chart xmlns:c="http://purl.oclc.org/ooxml/drawingml/chart" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
   <a:themeElements>
@@ -940,7 +1908,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H86"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
@@ -3172,11 +4140,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3187,8 +4155,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="d">
-        <v>2020-08-01</v>
+      <c r="A1" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>8</v>
@@ -3414,7 +4382,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added a test function for cumulative and new
</commit_message>
<xml_diff>
--- a/application/data/covid19_app_country_agnostic_dataset.xlsx
+++ b/application/data/covid19_app_country_agnostic_dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\University\COM618-DataScience\application\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{67741318-6BB6-42AF-B43A-80CFB8C4DA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{062311DF-2B74-45E3-AED1-009AC652E26D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3795" yWindow="1455" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid19_app_country_agnostic_da" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="11" uniqueCount="11">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="13" uniqueCount="13">
   <si>
     <t>Week starting</t>
   </si>
@@ -62,13 +62,19 @@
     <t>Cumulative number of NHS QR posters created</t>
   </si>
   <si>
-    <t>Downloads</t>
+    <t>Date</t>
   </si>
   <si>
-    <t>Deaths</t>
+    <t>new_downloads</t>
   </si>
   <si>
-    <t>Date</t>
+    <t>new_deaths</t>
+  </si>
+  <si>
+    <t>cumulative_downloads</t>
+  </si>
+  <si>
+    <t>cumulative_deaths</t>
   </si>
 </sst>
 </file>
@@ -1575,14 +1581,14 @@
 <xdr:wsDr xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>600074</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -4141,31 +4147,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="d">
         <v>2020-08-01</v>
       </c>
@@ -4176,8 +4190,16 @@
       <c r="C2" s="4">
         <v>297</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <f>SUM(B2+0)</f>
+        <v>107165</v>
+      </c>
+      <c r="E2">
+        <f>SUM(C2+0)</f>
+        <v>297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="d">
         <v>2020-09-01</v>
       </c>
@@ -4188,8 +4210,16 @@
       <c r="C3" s="5">
         <v>605</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <f>SUM(D2+B3)</f>
+        <v>14425885</v>
+      </c>
+      <c r="E3">
+        <f>SUM(E2+C3)</f>
+        <v>902</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="d">
         <v>2020-10-01</v>
       </c>
@@ -4200,8 +4230,16 @@
       <c r="C4" s="5">
         <v>3507</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <f t="shared" ref="D4:D19" si="0">SUM(D3+B4)</f>
+        <v>19201420</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E19" si="1">SUM(E3+C4)</f>
+        <v>4409</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="d">
         <v>2020-11-01</v>
       </c>
@@ -4212,8 +4250,16 @@
       <c r="C5" s="5">
         <v>8660</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>20169062</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>13069</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="d">
         <v>2020-12-01</v>
       </c>
@@ -4224,8 +4270,16 @@
       <c r="C6" s="5">
         <v>10678</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>21027032</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>23747</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="d">
         <v>2021-01-01</v>
       </c>
@@ -4236,8 +4290,16 @@
       <c r="C7" s="5">
         <v>19625</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>21318785</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>43372</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="d">
         <v>2021-02-01</v>
       </c>
@@ -4248,8 +4310,16 @@
       <c r="C8" s="5">
         <v>9532</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>21610538</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>52904</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="d">
         <v>2021-03-01</v>
       </c>
@@ -4260,8 +4330,16 @@
       <c r="C9" s="5">
         <v>2853</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>21961457</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>55757</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="d">
         <v>2021-04-01</v>
       </c>
@@ -4272,8 +4350,16 @@
       <c r="C10" s="5">
         <v>713</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>22999216</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>56470</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="d">
         <v>2021-05-01</v>
       </c>
@@ -4284,8 +4370,16 @@
       <c r="C11" s="5">
         <v>273</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>24212888</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>56743</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="d">
         <v>2021-06-01</v>
       </c>
@@ -4296,8 +4390,16 @@
       <c r="C12" s="5">
         <v>329</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>25845805</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>57072</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="d">
         <v>2021-07-01</v>
       </c>
@@ -4308,8 +4410,16 @@
       <c r="C13" s="5">
         <v>1218</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>26956127</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>58290</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="d">
         <v>2021-08-01</v>
       </c>
@@ -4320,8 +4430,16 @@
       <c r="C14" s="5">
         <v>2346</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>27394039</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>60636</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="d">
         <v>2021-09-01</v>
       </c>
@@ -4332,8 +4450,16 @@
       <c r="C15" s="5">
         <v>2741</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>27915022</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>63377</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="d">
         <v>2021-10-01</v>
       </c>
@@ -4344,8 +4470,16 @@
       <c r="C16" s="5">
         <v>2809</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>28258692</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>66186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="d">
         <v>2021-11-01</v>
       </c>
@@ -4356,8 +4490,16 @@
       <c r="C17" s="5">
         <v>3002</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>28601672</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>69188</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="d">
         <v>2021-12-01</v>
       </c>
@@ -4368,8 +4510,16 @@
       <c r="C18" s="5">
         <v>2958</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>29352760</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>72146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="d">
         <v>2022-01-01</v>
       </c>
@@ -4379,6 +4529,14 @@
       </c>
       <c r="C19" s="5">
         <v>4292</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>29890542</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>76438</v>
       </c>
     </row>
   </sheetData>

</xml_diff>